<commit_message>
updated prog languages and upversioned code
</commit_message>
<xml_diff>
--- a/original-table.xlsx
+++ b/original-table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\acm.timus_artemiy_lessons\2023\from-table-to-oop-cs\ConsoleApp1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C538A8CD-E2B9-4239-A231-E634F304789F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3908917F-9A2A-4D91-906A-1C11CB651EBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3D1E1B0C-DC54-497A-932F-ECFDAA494525}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="86">
   <si>
     <t>Название</t>
   </si>
@@ -163,16 +163,152 @@
   </si>
   <si>
     <t>2014</t>
+  </si>
+  <si>
+    <t>Джеймс Гослинг</t>
+  </si>
+  <si>
+    <t>Java SE 19.0.1</t>
+  </si>
+  <si>
+    <t>18.10.2022</t>
+  </si>
+  <si>
+    <t>Крис Латтнер</t>
+  </si>
+  <si>
+    <t>5.7.2</t>
+  </si>
+  <si>
+    <t>14.12.2022</t>
+  </si>
+  <si>
+    <t>Джеймс Стрэкан</t>
+  </si>
+  <si>
+    <t>4.0.7</t>
+  </si>
+  <si>
+    <t>21.12.2022</t>
+  </si>
+  <si>
+    <t>Perl</t>
+  </si>
+  <si>
+    <t>Rust</t>
+  </si>
+  <si>
+    <t>1.19.4</t>
+  </si>
+  <si>
+    <t>06.12.2022</t>
+  </si>
+  <si>
+    <t>Роберт Гризмер, Роб Пайк и Кен Томпсон</t>
+  </si>
+  <si>
+    <t>3.1.3</t>
+  </si>
+  <si>
+    <t>Мартин Одерски</t>
+  </si>
+  <si>
+    <t>21.06.2022</t>
+  </si>
+  <si>
+    <t>8.2.0</t>
+  </si>
+  <si>
+    <t>Расмус Лердорф, Энди Гутманс</t>
+  </si>
+  <si>
+    <t>08.12.2022</t>
+  </si>
+  <si>
+    <t>3.2.0</t>
+  </si>
+  <si>
+    <t>25.12.2022</t>
+  </si>
+  <si>
+    <t>Юкихиро Мацумото</t>
+  </si>
+  <si>
+    <t>Бред Кокс</t>
+  </si>
+  <si>
+    <t>2.0</t>
+  </si>
+  <si>
+    <t>19.10.2022</t>
+  </si>
+  <si>
+    <t>Леннарт Аугустссон, Уоррен Бертон</t>
+  </si>
+  <si>
+    <t>Haskell 2010</t>
+  </si>
+  <si>
+    <t>01.07.2010</t>
+  </si>
+  <si>
+    <t>Бьёрн Страуструп</t>
+  </si>
+  <si>
+    <t>C++20</t>
+  </si>
+  <si>
+    <t>01.12.2020</t>
+  </si>
+  <si>
+    <t>Брендан Эйх</t>
+  </si>
+  <si>
+    <t>ECMAScript 2022</t>
+  </si>
+  <si>
+    <t>01.06.2022</t>
+  </si>
+  <si>
+    <t>1987</t>
+  </si>
+  <si>
+    <t>5.36.0</t>
+  </si>
+  <si>
+    <t>28.05.2022</t>
+  </si>
+  <si>
+    <t>Ларри Уолл</t>
+  </si>
+  <si>
+    <t>Грэйдон Хор</t>
+  </si>
+  <si>
+    <t>2006</t>
+  </si>
+  <si>
+    <t>1.66.1</t>
+  </si>
+  <si>
+    <t>10.01.2023</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -524,44 +660,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9FD2D85-D652-4048-9068-D4240F92E62F}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.77734375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.77734375" style="3" customWidth="1"/>
-    <col min="3" max="9" width="13.77734375" style="1" customWidth="1"/>
+    <col min="1" max="7" width="13.77734375" style="3" customWidth="1"/>
+    <col min="8" max="9" width="13.77734375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="3">
@@ -585,7 +720,7 @@
       <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="3">
@@ -609,7 +744,7 @@
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="3">
@@ -633,7 +768,7 @@
       <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="3">
@@ -656,95 +791,307 @@
       </c>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B6" s="3">
         <v>1995</v>
       </c>
+      <c r="C6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="3" t="s">
         <v>41</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="C7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="C8" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+      <c r="C9" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+      <c r="C10" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+      <c r="C11" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>33</v>
       </c>
+      <c r="C12" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+      <c r="C13" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+      <c r="C14" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
+      <c r="C15" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B16" s="3">
         <v>1996</v>
       </c>
+      <c r="C16" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>85</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>